<commit_message>
DOCS - update readme
</commit_message>
<xml_diff>
--- a/DOCS/Documentação das Sprints/burn2.xlsx
+++ b/DOCS/Documentação das Sprints/burn2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\FATEC\sem2\API-2\DOCS\Documentação das Sprints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01EEC194-4282-4BBE-A6EA-AD99708F024D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72669CA9-52A3-4744-B0CC-FC25136AC257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -2442,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>